<commit_message>
published state of ETDataset on 16 January 2018
</commit_message>
<xml_diff>
--- a/supporting_data/local/rietdiep/Area (Reitdiep - Groningen).xlsx
+++ b/supporting_data/local/rietdiep/Area (Reitdiep - Groningen).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-10360" windowWidth="51200" windowHeight="28360" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="28800" yWindow="-10360" windowWidth="25600" windowHeight="28360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -802,7 +802,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -880,7 +880,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1513,8 +1512,8 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1707,7 +1706,7 @@
       <c r="E12" s="27"/>
       <c r="F12" s="26"/>
       <c r="G12" s="26"/>
-      <c r="H12" s="57" t="s">
+      <c r="H12" s="56" t="s">
         <v>163</v>
       </c>
       <c r="I12" s="4"/>
@@ -2169,8 +2168,8 @@
       <c r="E34" s="1">
         <v>154.69</v>
       </c>
-      <c r="F34" s="49">
-        <v>1.0694779999999999E-2</v>
+      <c r="F34">
+        <v>1.090085E-2</v>
       </c>
       <c r="H34" s="19" t="s">
         <v>160</v>
@@ -2684,7 +2683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+    <sheetView zoomScale="87" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -2695,7 +2694,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="49" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2781,160 +2780,160 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="51"/>
-      <c r="B10" s="51"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
+      <c r="A10" s="50"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="52">
+      <c r="C11" s="51">
         <f>[1]Dashboard!F23</f>
         <v>918</v>
       </c>
-      <c r="D11" s="51" t="s">
+      <c r="D11" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="E11" s="51"/>
+      <c r="E11" s="50"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="53">
+      <c r="C12" s="52">
         <f>[1]Dashboard!F24</f>
         <v>160</v>
       </c>
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="E12" s="51"/>
+      <c r="E12" s="50"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="50" t="s">
         <v>124</v>
       </c>
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="54">
+      <c r="C13" s="53">
         <f>SUM(C11:C12)</f>
         <v>1078</v>
       </c>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="51"/>
-      <c r="B14" s="51"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
+      <c r="A14" s="50"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="51"/>
-      <c r="B15" s="51"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
+      <c r="A15" s="50"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="51"/>
-      <c r="B16" s="51"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="51"/>
+      <c r="A16" s="50"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="50" t="s">
+      <c r="A43" s="49" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="55"/>
-      <c r="B44" s="55" t="s">
+      <c r="A44" s="54"/>
+      <c r="B44" s="54" t="s">
         <v>112</v>
       </c>
-      <c r="C44" s="55"/>
-      <c r="D44" s="55" t="s">
+      <c r="C44" s="54"/>
+      <c r="D44" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="E44" s="55"/>
-      <c r="F44" s="55"/>
+      <c r="E44" s="54"/>
+      <c r="F44" s="54"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="55" t="s">
+      <c r="A45" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="B45" s="55" t="s">
+      <c r="B45" s="54" t="s">
         <v>119</v>
       </c>
-      <c r="C45" s="55">
+      <c r="C45" s="54">
         <v>1000000</v>
       </c>
-      <c r="D45" s="55"/>
-      <c r="E45" s="55"/>
-      <c r="F45" s="55"/>
+      <c r="D45" s="54"/>
+      <c r="E45" s="54"/>
+      <c r="F45" s="54"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="56" t="s">
+      <c r="A46" s="55" t="s">
         <v>125</v>
       </c>
       <c r="B46" t="s">
         <v>25</v>
       </c>
-      <c r="C46" s="55" t="s">
+      <c r="C46" s="54" t="s">
         <v>128</v>
       </c>
-      <c r="D46" s="55" t="s">
+      <c r="D46" s="54" t="s">
         <v>30</v>
       </c>
       <c r="E46" t="s">
         <v>129</v>
       </c>
-      <c r="F46" s="55"/>
+      <c r="F46" s="54"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="56" t="s">
+      <c r="A47" s="55" t="s">
         <v>125</v>
       </c>
-      <c r="B47" s="55" t="s">
+      <c r="B47" s="54" t="s">
         <v>119</v>
       </c>
-      <c r="C47" s="55">
+      <c r="C47" s="54">
         <v>51849.63</v>
       </c>
-      <c r="D47" s="55" t="s">
+      <c r="D47" s="54" t="s">
         <v>130</v>
       </c>
-      <c r="E47" s="55" t="s">
+      <c r="E47" s="54" t="s">
         <v>131</v>
       </c>
-      <c r="F47" s="55"/>
+      <c r="F47" s="54"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="55" t="s">
+      <c r="A48" s="54" t="s">
         <v>132</v>
       </c>
-      <c r="B48" s="55" t="s">
+      <c r="B48" s="54" t="s">
         <v>133</v>
       </c>
-      <c r="C48" s="55">
+      <c r="C48" s="54">
         <f>C47/C45</f>
         <v>5.1849630000000001E-2</v>
       </c>
-      <c r="D48" s="55"/>
-      <c r="E48" s="55"/>
-      <c r="F48" s="55"/>
+      <c r="D48" s="54"/>
+      <c r="E48" s="54"/>
+      <c r="F48" s="54"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4195,11 +4194,11 @@
       </c>
       <c r="D73">
         <f>Dashboard!F34</f>
-        <v>1.0694779999999999E-2</v>
+        <v>1.090085E-2</v>
       </c>
       <c r="E73" t="str">
         <f t="shared" si="7"/>
-        <v>- co2_emission_1990 = 0.01069478</v>
+        <v>- co2_emission_1990 = 0.01090085</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>